<commit_message>
Updated data and graph 9 buggy
</commit_message>
<xml_diff>
--- a/Anna Plots/Ice Mass Data.xlsx
+++ b/Anna Plots/Ice Mass Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\University UT\Year 4 Courses\STA313\STA313 Github\DataVisProject\Anna Plots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\University UT\Year 4 Courses\Winter STA313\STA313 Github\DataVisProject\Anna Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2846E1B-489A-4826-9132-788A463D419A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF40AB3-B83D-4367-8D91-3D618B55ABD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11652" yWindow="384" windowWidth="10884" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1384,7 +1384,7 @@
   <dimension ref="A1:H195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>